<commit_message>
updated tests and API
</commit_message>
<xml_diff>
--- a/core/excel/src/test/resources/example.xlsx
+++ b/core/excel/src/test/resources/example.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Employees" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
   <si>
     <t>Peter</t>
   </si>
@@ -23,6 +24,12 @@
   </si>
   <si>
     <t>Quality Assurance</t>
+  </si>
+  <si>
+    <t>Die</t>
+  </si>
+  <si>
+    <t>Director</t>
   </si>
 </sst>
 </file>
@@ -170,6 +177,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -211,4 +222,61 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>